<commit_message>
get back to working car; fix logic errors; todo save history
</commit_message>
<xml_diff>
--- a/sensorsData.xlsx
+++ b/sensorsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkhalzov/Documents/PlatformIO/Projects/190602-140824-uno/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E55C5C9C-4F6F-9D4A-B380-083A8729952C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7E060136-B1C9-1447-AB59-070FEF920C7E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28600" windowHeight="16540" activeTab="1"/>
   </bookViews>
@@ -16,12 +16,20 @@
     <sheet name="sensorsData" sheetId="1" r:id="rId1"/>
     <sheet name="sensorsData (2)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="8">
   <si>
     <t>State: Initial setup</t>
   </si>
@@ -42,6 +50,9 @@
   </si>
   <si>
     <t>Speed up</t>
+  </si>
+  <si>
+    <t>Max value</t>
   </si>
 </sst>
 </file>
@@ -7408,8 +7419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7972,10 +7983,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D104"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8592,7 +8603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>125</v>
       </c>
@@ -8606,7 +8617,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>118</v>
       </c>
@@ -8620,7 +8631,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>119</v>
       </c>
@@ -8634,7 +8645,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>117</v>
       </c>
@@ -8648,12 +8659,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>125</v>
       </c>
@@ -8667,7 +8678,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>135</v>
       </c>
@@ -8681,7 +8692,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>146</v>
       </c>
@@ -8695,7 +8706,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>152</v>
       </c>
@@ -8709,7 +8720,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>158</v>
       </c>
@@ -8723,7 +8734,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>163</v>
       </c>
@@ -8737,7 +8748,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>166</v>
       </c>
@@ -8751,12 +8762,12 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>170</v>
       </c>
@@ -8769,8 +8780,15 @@
       <c r="D62" s="4">
         <v>179</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F62" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62">
+        <f>MAX(A1:D104)</f>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>175</v>
       </c>
@@ -8784,7 +8802,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>175</v>
       </c>

</xml_diff>